<commit_message>
Improving spreadsheet, including data file
</commit_message>
<xml_diff>
--- a/data/excelsheets/nspsurveydata.xlsx
+++ b/data/excelsheets/nspsurveydata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4809" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4809" uniqueCount="340">
   <si>
     <t>Time since first injection</t>
   </si>
@@ -882,6 +882,171 @@
   <si>
     <t>Teleprevir/Boceprevir&amp;INF-RBV</t>
   </si>
+  <si>
+    <t>14  to 54</t>
+  </si>
+  <si>
+    <t>13  to 59</t>
+  </si>
+  <si>
+    <t>15  to 58</t>
+  </si>
+  <si>
+    <t>14  to 63</t>
+  </si>
+  <si>
+    <t>14  to 69</t>
+  </si>
+  <si>
+    <t>14  to 61</t>
+  </si>
+  <si>
+    <t>14  to 62</t>
+  </si>
+  <si>
+    <t>15  to 64</t>
+  </si>
+  <si>
+    <t>16  to 65</t>
+  </si>
+  <si>
+    <t>15  to 66</t>
+  </si>
+  <si>
+    <t>13  to 68</t>
+  </si>
+  <si>
+    <t>16  to 70</t>
+  </si>
+  <si>
+    <t>15  to 73</t>
+  </si>
+  <si>
+    <t>10  to 48</t>
+  </si>
+  <si>
+    <t>10  to 50</t>
+  </si>
+  <si>
+    <t>10  to 47</t>
+  </si>
+  <si>
+    <t>10  to 55</t>
+  </si>
+  <si>
+    <t>10  to 54</t>
+  </si>
+  <si>
+    <t>10  to 53</t>
+  </si>
+  <si>
+    <t>10  to 56</t>
+  </si>
+  <si>
+    <t>10  to 52</t>
+  </si>
+  <si>
+    <t>10  to 60</t>
+  </si>
+  <si>
+    <t>10  to 58</t>
+  </si>
+  <si>
+    <t>10  to 63</t>
+  </si>
+  <si>
+    <t>&lt;1  to 33</t>
+  </si>
+  <si>
+    <t>&lt;1  to 37</t>
+  </si>
+  <si>
+    <t>&lt;1  to 40</t>
+  </si>
+  <si>
+    <t>&lt;1  to 36</t>
+  </si>
+  <si>
+    <t>&lt;1  to 41</t>
+  </si>
+  <si>
+    <t>&lt;1  to 44</t>
+  </si>
+  <si>
+    <t>&lt;1  to 43</t>
+  </si>
+  <si>
+    <t>&lt;1  to 45</t>
+  </si>
+  <si>
+    <t>&lt;1  to 46</t>
+  </si>
+  <si>
+    <t>&lt;1  to 49</t>
+  </si>
+  <si>
+    <t>&lt;1  to 48</t>
+  </si>
+  <si>
+    <t>Non  to English </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re  to used someone else’s used needle &amp; syringe last month (%) </t>
+  </si>
+  <si>
+    <t>3  to 5times</t>
+  </si>
+  <si>
+    <t>Number of people needle &amp; syringe was re  to used after last month (%)</t>
+  </si>
+  <si>
+    <t>Table 1.28 HCV antibody prevalence by re  to use of someone else’s used needle and syringe last month, time since first injection and year  </t>
+  </si>
+  <si>
+    <t>Table 1.1 NSP 1995  to 2010</t>
+  </si>
+  <si>
+    <t>16  to 71</t>
+  </si>
+  <si>
+    <t>15  to 67</t>
+  </si>
+  <si>
+    <t>10  to 70</t>
+  </si>
+  <si>
+    <t>10  to 61</t>
+  </si>
+  <si>
+    <t>&lt;1  to 53</t>
+  </si>
+  <si>
+    <t>&lt;1  to 51</t>
+  </si>
+  <si>
+    <t>Teleprevir/Boceprevir&amp;INF  to RBV*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interferon+/orRibavirin   to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  to  </t>
+  </si>
+  <si>
+    <t>Teleprevir/Boceprevir&amp;INF  to RBV</t>
+  </si>
+  <si>
+    <t>History of buprenorphine  to naloxone (Suboxone®) treatment (%)</t>
+  </si>
+  <si>
+    <t>25  to 34years</t>
+  </si>
+  <si>
+    <t>3  to 10years</t>
+  </si>
+  <si>
+    <t>&lt;1  to 60</t>
+  </si>
 </sst>
 </file>
 
@@ -1255,10 +1420,10 @@
   <dimension ref="A1:T388"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B352" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B347" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A259" sqref="A259:T388"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1495,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1973,61 +2138,61 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>285</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>286</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>287</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>288</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>289</v>
       </c>
       <c r="G16" t="s">
-        <v>20</v>
+        <v>290</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>291</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>288</v>
       </c>
       <c r="J16" t="s">
-        <v>22</v>
+        <v>292</v>
       </c>
       <c r="K16" t="s">
-        <v>23</v>
+        <v>293</v>
       </c>
       <c r="L16" t="s">
-        <v>24</v>
+        <v>294</v>
       </c>
       <c r="M16" t="s">
-        <v>25</v>
+        <v>295</v>
       </c>
       <c r="N16" t="s">
-        <v>19</v>
+        <v>289</v>
       </c>
       <c r="O16" t="s">
-        <v>26</v>
+        <v>296</v>
       </c>
       <c r="P16" t="s">
-        <v>24</v>
+        <v>294</v>
       </c>
       <c r="Q16" t="s">
-        <v>27</v>
+        <v>297</v>
       </c>
       <c r="R16" t="s">
-        <v>171</v>
+        <v>293</v>
       </c>
       <c r="S16" t="s">
-        <v>172</v>
+        <v>326</v>
       </c>
       <c r="T16" t="s">
-        <v>173</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -2288,61 +2453,61 @@
         <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>298</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>298</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>299</v>
       </c>
       <c r="E23" t="s">
-        <v>31</v>
+        <v>300</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>301</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>302</v>
       </c>
       <c r="H23" t="s">
-        <v>34</v>
+        <v>303</v>
       </c>
       <c r="I23" t="s">
-        <v>35</v>
+        <v>304</v>
       </c>
       <c r="J23" t="s">
-        <v>30</v>
+        <v>299</v>
       </c>
       <c r="K23" t="s">
-        <v>35</v>
+        <v>304</v>
       </c>
       <c r="L23" t="s">
-        <v>32</v>
+        <v>301</v>
       </c>
       <c r="M23" t="s">
-        <v>36</v>
+        <v>305</v>
       </c>
       <c r="N23" t="s">
-        <v>35</v>
+        <v>304</v>
       </c>
       <c r="O23" t="s">
-        <v>37</v>
+        <v>306</v>
       </c>
       <c r="P23" t="s">
-        <v>38</v>
+        <v>307</v>
       </c>
       <c r="Q23" t="s">
-        <v>39</v>
+        <v>308</v>
       </c>
       <c r="R23" t="s">
-        <v>177</v>
+        <v>304</v>
       </c>
       <c r="S23" t="s">
-        <v>178</v>
+        <v>328</v>
       </c>
       <c r="T23" t="s">
-        <v>179</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -2474,61 +2639,61 @@
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>309</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>310</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>310</v>
       </c>
       <c r="E27" t="s">
-        <v>43</v>
+        <v>311</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>312</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>313</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>314</v>
       </c>
       <c r="I27" t="s">
-        <v>47</v>
+        <v>315</v>
       </c>
       <c r="J27" t="s">
-        <v>48</v>
+        <v>316</v>
       </c>
       <c r="K27" t="s">
-        <v>49</v>
+        <v>317</v>
       </c>
       <c r="L27" t="s">
-        <v>49</v>
+        <v>317</v>
       </c>
       <c r="M27" t="s">
-        <v>48</v>
+        <v>316</v>
       </c>
       <c r="N27" t="s">
-        <v>50</v>
+        <v>318</v>
       </c>
       <c r="O27" t="s">
-        <v>51</v>
+        <v>319</v>
       </c>
       <c r="P27" t="s">
-        <v>49</v>
+        <v>317</v>
       </c>
       <c r="Q27" t="s">
-        <v>52</v>
+        <v>339</v>
       </c>
       <c r="R27" t="s">
-        <v>174</v>
+        <v>313</v>
       </c>
       <c r="S27" t="s">
-        <v>175</v>
+        <v>330</v>
       </c>
       <c r="T27" t="s">
-        <v>176</v>
+        <v>331</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -3359,7 +3524,7 @@
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>320</v>
       </c>
       <c r="B45" t="s">
         <v>94</v>
@@ -4560,25 +4725,25 @@
         <v>90</v>
       </c>
       <c r="B69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I69">
         <v>25</v>
@@ -6029,7 +6194,7 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>321</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
@@ -6220,7 +6385,7 @@
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>322</v>
       </c>
       <c r="B105">
         <v>71</v>
@@ -6406,7 +6571,7 @@
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>103</v>
+        <v>323</v>
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
@@ -11334,7 +11499,7 @@
     </row>
     <row r="213" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>283</v>
+        <v>332</v>
       </c>
       <c r="B213" t="s">
         <v>94</v>
@@ -11637,13 +11802,13 @@
     </row>
     <row r="219" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>280</v>
+        <v>333</v>
       </c>
       <c r="B219" t="s">
         <v>94</v>
       </c>
       <c r="C219" t="s">
-        <v>95</v>
+        <v>334</v>
       </c>
       <c r="D219" t="s">
         <v>94</v>
@@ -11699,7 +11864,7 @@
     </row>
     <row r="220" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>284</v>
+        <v>335</v>
       </c>
       <c r="B220" t="s">
         <v>94</v>
@@ -12840,7 +13005,7 @@
     </row>
     <row r="244" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>255</v>
+        <v>336</v>
       </c>
     </row>
     <row r="245" spans="1:20" x14ac:dyDescent="0.25">
@@ -13171,7 +13336,7 @@
         <v>94</v>
       </c>
       <c r="C253" t="s">
-        <v>95</v>
+        <v>334</v>
       </c>
       <c r="D253" t="s">
         <v>94</v>
@@ -15861,7 +16026,7 @@
     </row>
     <row r="308" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A308" s="5" t="s">
-        <v>231</v>
+        <v>337</v>
       </c>
       <c r="B308" s="5">
         <v>296</v>
@@ -16257,7 +16422,7 @@
     </row>
     <row r="315" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
-        <v>231</v>
+        <v>337</v>
       </c>
       <c r="B315" s="5">
         <v>136</v>
@@ -16653,7 +16818,7 @@
     </row>
     <row r="322" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A322" s="5" t="s">
-        <v>231</v>
+        <v>337</v>
       </c>
       <c r="B322" s="5">
         <v>435</v>
@@ -17095,7 +17260,7 @@
     </row>
     <row r="331" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A331" s="5" t="s">
-        <v>240</v>
+        <v>338</v>
       </c>
       <c r="B331" s="5">
         <v>229</v>
@@ -17491,7 +17656,7 @@
     </row>
     <row r="338" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A338" s="5" t="s">
-        <v>240</v>
+        <v>338</v>
       </c>
       <c r="B338" s="5">
         <v>141</v>
@@ -17887,7 +18052,7 @@
     </row>
     <row r="345" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A345" s="5" t="s">
-        <v>240</v>
+        <v>338</v>
       </c>
       <c r="B345" s="5">
         <v>375</v>
@@ -19391,7 +19556,7 @@
     </row>
     <row r="373" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A373" s="5" t="s">
-        <v>252</v>
+        <v>324</v>
       </c>
       <c r="B373" s="5"/>
       <c r="C373" s="5"/>

</xml_diff>